<commit_message>
update plenty of plots
</commit_message>
<xml_diff>
--- a/output/tables.xlsx
+++ b/output/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/GitHub/covid_wildfire/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3319A9D-7DBC-2843-85F2-337298450B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBF7530-D237-1845-94BD-DDB9F854F7AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="480" windowWidth="27940" windowHeight="19660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9020" yWindow="680" windowWidth="27940" windowHeight="19660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="137">
   <si>
     <t>var</t>
   </si>
@@ -221,9 +221,6 @@
     <t>21,808 (85.0%)</t>
   </si>
   <si>
-    <t>Mean of Daily PM2.5 (ug/m3)</t>
-  </si>
-  <si>
     <t>15 (0 - 89)</t>
   </si>
   <si>
@@ -291,16 +288,194 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t># Day with zero death</t>
+  </si>
+  <si>
+    <t># Day with zero case</t>
+  </si>
+  <si>
+    <t># Total Day with zero case</t>
+  </si>
+  <si>
+    <t># Total Day with zero death</t>
+  </si>
+  <si>
+    <t>Daily Cases</t>
+  </si>
+  <si>
+    <t>Daily Deaths</t>
+  </si>
+  <si>
+    <t>9.7 (11.0%)</t>
+  </si>
+  <si>
+    <t>78.3 (89.0%)</t>
+  </si>
+  <si>
+    <t>23.2 (10.7%)</t>
+  </si>
+  <si>
+    <t>31.2 (11.3%)</t>
+  </si>
+  <si>
+    <t>245.8 (88.7%)</t>
+  </si>
+  <si>
+    <t>193.8 (89.3%)</t>
+  </si>
+  <si>
+    <t>Number of Days</t>
+  </si>
+  <si>
+    <t>31 (16.8 - 43.2)</t>
+  </si>
+  <si>
+    <t>246 (233.8 - 260.2)</t>
+  </si>
+  <si>
+    <t>11.2% (6.0% - 15.6%)</t>
+  </si>
+  <si>
+    <t>88.8% (84.4% - 94.0%)</t>
+  </si>
+  <si>
+    <t>65 (54.0 - 93.0)</t>
+  </si>
+  <si>
+    <t>3.5 (0.0 - 11.8)</t>
+  </si>
+  <si>
+    <t>58 (44.0 - 85.5)</t>
+  </si>
+  <si>
+    <t>260 (199.0 - 270.5)</t>
+  </si>
+  <si>
+    <t>93.9% (71.8% - 97.6%)</t>
+  </si>
+  <si>
+    <t>19 (12.5 - 36.5)</t>
+  </si>
+  <si>
+    <t>6.9% (4.5% - 13.2%)</t>
+  </si>
+  <si>
+    <t>215.5 (168.8 - 232.8)</t>
+  </si>
+  <si>
+    <t>77.8% (60.9% - 84.0%)</t>
+  </si>
+  <si>
+    <t>% Number of Days</t>
+  </si>
+  <si>
+    <t>%Day with zero death</t>
+  </si>
+  <si>
+    <t>15.0 (4.4 - 66.9)</t>
+  </si>
+  <si>
+    <t>15.4 (2.6 - 40.0)</t>
+  </si>
+  <si>
+    <t>15.2 (4.4, 64.3)</t>
+  </si>
+  <si>
+    <t>0.18 (0.00 - 0.87)</t>
+  </si>
+  <si>
+    <t>0.15 (0.05 - 0.70)</t>
+  </si>
+  <si>
+    <t>9.8 (7.3 - 15.9)</t>
+  </si>
+  <si>
+    <t>7.9 (3.9 - 13.7)</t>
+  </si>
+  <si>
+    <t>10.0 (7.3 - 16.0)</t>
+  </si>
+  <si>
+    <t>Percent of Days with zero COVID19 case</t>
+  </si>
+  <si>
+    <t>Percent of Days with zero COVID19 death</t>
+  </si>
+  <si>
+    <t>Daily PM2.5 (\mu g/m^3)</t>
+  </si>
+  <si>
+    <t>Daily Cases Rate (per 100,000)</t>
+  </si>
+  <si>
+    <t>Daily Deaths Rate (per 1,000,000)</t>
+  </si>
+  <si>
+    <t>5.5 (2.0 - 35.4)</t>
+  </si>
+  <si>
+    <t>26.4 (4.8 - 195.8)</t>
+  </si>
+  <si>
+    <t>5.0 (1.9 - 15.9)</t>
+  </si>
+  <si>
+    <t>26.5% (13.5% - 45.1%)</t>
+  </si>
+  <si>
+    <t>23.6% (4.8% - 36.7%)</t>
+  </si>
+  <si>
+    <t>27.1% (13.7% - 46.6%)</t>
+  </si>
+  <si>
+    <t>87.7%(63.6% - 95.1%)</t>
+  </si>
+  <si>
+    <t>84.6% (56.2% - 98.8%)</t>
+  </si>
+  <si>
+    <t>88.7% (65.3% - 95.7%)</t>
+  </si>
+  <si>
+    <t>1.23 (0.42 - 3.05)</t>
+  </si>
+  <si>
+    <t>1.25 (0.00 - 5.91)</t>
+  </si>
+  <si>
+    <t>1.13 (0.44 - 2.96)</t>
+  </si>
+  <si>
+    <t>26.5 (13.5 - 45.1)</t>
+  </si>
+  <si>
+    <t>23.6 (4.8 - 36.7)</t>
+  </si>
+  <si>
+    <t>27.1 (13.7 - 46.6)</t>
+  </si>
+  <si>
+    <t>87.7(63.6 - 95.1)</t>
+  </si>
+  <si>
+    <t>84.6 (56.2 - 98.8)</t>
+  </si>
+  <si>
+    <t>88.7 (65.3 - 95.7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,6 +606,19 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -812,7 +1000,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -838,10 +1026,6 @@
     <xf numFmtId="3" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,13 +1041,48 @@
     <xf numFmtId="3" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1221,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2132,8 +2351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B04A5A0-7B2E-EC49-8345-03587248DDE7}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2163,13 +2382,13 @@
         <v>46</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -2177,19 +2396,19 @@
         <v>41</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -2203,13 +2422,13 @@
         <v>36</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -2217,19 +2436,19 @@
         <v>43</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -2243,18 +2462,18 @@
         <v>36</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="F8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2">
         <v>277</v>
@@ -2262,42 +2481,42 @@
     </row>
     <row r="10" spans="2:12" ht="19" customHeight="1">
       <c r="H10" s="5"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20" t="s">
+      <c r="K10" s="17"/>
+      <c r="L10" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="19" customHeight="1">
       <c r="H11" s="3"/>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="21"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="2:12">
       <c r="H12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="14">
         <v>78.3</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="14">
         <v>4.5</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="14">
         <v>73.900000000000006</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="13">
         <v>5.3</v>
       </c>
     </row>
@@ -2305,16 +2524,16 @@
       <c r="H13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="14">
         <v>66.099999999999994</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="14">
         <v>7</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="14">
         <v>59</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="13">
         <v>6</v>
       </c>
     </row>
@@ -2322,16 +2541,16 @@
       <c r="H14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="14">
         <v>42.9</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="14">
         <v>8.9</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="14">
         <v>34</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="14">
         <v>8</v>
       </c>
     </row>
@@ -2340,16 +2559,16 @@
       <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="15">
         <v>52.9</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="15">
         <v>7.8</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="15">
         <v>45</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="15">
         <v>6.6</v>
       </c>
     </row>
@@ -2359,23 +2578,23 @@
     <row r="17" spans="6:12">
       <c r="F17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L17" s="2">
         <v>277</v>
       </c>
     </row>
     <row r="18" spans="6:12">
-      <c r="I18" s="22"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="6:12">
-      <c r="I19" s="22"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="6:12">
-      <c r="I20" s="22"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="6:12">
-      <c r="I21" s="22"/>
+      <c r="I21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2387,131 +2606,643 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A2DA9A-C4CC-3B47-ADFD-0F194D4ADFA0}">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="4.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="24.83203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="28" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="B2" s="5"/>
-      <c r="C2" s="10" t="s">
+    <row r="1" spans="2:7" s="23" customFormat="1">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="2:7" s="23" customFormat="1">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:7" s="23" customFormat="1">
+      <c r="B3" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="27">
+        <v>25484</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="2:7" s="23" customFormat="1">
+      <c r="B4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1929511</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="2:7" s="23" customFormat="1">
+      <c r="B5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="29">
+        <v>25654</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="2:7" s="23" customFormat="1">
+      <c r="B6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="32">
+        <v>11.8</v>
+      </c>
+      <c r="D6" s="32">
+        <v>52.9</v>
+      </c>
+      <c r="E6" s="32">
+        <v>6.6</v>
+      </c>
+      <c r="F6" s="33"/>
+    </row>
+    <row r="7" spans="2:7" s="23" customFormat="1">
+      <c r="B7" s="28"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="2:7" s="23" customFormat="1">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="33"/>
+    </row>
+    <row r="9" spans="2:7" s="23" customFormat="1">
+      <c r="B9" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="30">
+        <v>277</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" spans="2:7" s="23" customFormat="1">
+      <c r="B10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="34">
+        <v>88</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="2:7" s="23" customFormat="1">
+      <c r="B11" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="34">
+        <v>217.04347826086956</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7" s="23" customFormat="1">
+      <c r="B12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="24">
+        <v>76.2</v>
+      </c>
+      <c r="D12" s="35">
+        <v>61.4</v>
+      </c>
+      <c r="E12" s="35">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="23" customFormat="1">
+      <c r="B13" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="30">
+        <v>1.01</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1.34</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0.96</v>
+      </c>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="2:7" s="23" customFormat="1">
+      <c r="B14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="32">
+        <v>11.8</v>
+      </c>
+      <c r="D14" s="32">
+        <v>52.9</v>
+      </c>
+      <c r="E14" s="32">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="23" customFormat="1">
+      <c r="B15" s="28"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="2:7" s="23" customFormat="1">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="23" customFormat="1">
+      <c r="B17" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="30">
+        <v>277</v>
+      </c>
+      <c r="D17" s="30">
+        <v>31.2</v>
+      </c>
+      <c r="E17" s="30">
+        <v>245.8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="23" customFormat="1">
+      <c r="B18" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="34">
+        <v>88</v>
+      </c>
+      <c r="D18" s="34">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E18" s="34">
+        <v>78.3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="23" customFormat="1">
+      <c r="B19" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="34">
+        <v>217.04347826086956</v>
+      </c>
+      <c r="D19" s="34">
+        <v>23.2</v>
+      </c>
+      <c r="E19" s="34">
+        <v>193.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="23" customFormat="1">
+      <c r="B20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="24">
+        <v>76.2</v>
+      </c>
+      <c r="D20" s="35">
+        <v>61.4</v>
+      </c>
+      <c r="E20" s="35">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="23" customFormat="1">
+      <c r="B21" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="30">
+        <v>1.01</v>
+      </c>
+      <c r="D21" s="30">
+        <v>1.34</v>
+      </c>
+      <c r="E21" s="30">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="23" customFormat="1">
+      <c r="B22" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="32">
+        <v>11.8</v>
+      </c>
+      <c r="D22" s="32">
+        <v>52.9</v>
+      </c>
+      <c r="E22" s="32">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="23" customFormat="1">
+      <c r="B23" s="30"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="H23" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="12">
-        <v>25484</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1929511</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="13">
-        <v>25654</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="9">
-        <v>11.8</v>
-      </c>
-      <c r="D6" s="9">
-        <v>52.9</v>
-      </c>
-      <c r="E6" s="9">
-        <v>6.6</v>
-      </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
+    </row>
+    <row r="24" spans="2:8" s="23" customFormat="1">
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="2:8" s="23" customFormat="1">
+      <c r="B25" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="30">
+        <v>8096</v>
+      </c>
+      <c r="D25" s="30">
+        <v>889</v>
+      </c>
+      <c r="E25" s="30">
+        <v>7207</v>
+      </c>
+      <c r="F25" s="33"/>
+    </row>
+    <row r="26" spans="2:8" s="23" customFormat="1">
+      <c r="B26" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="30">
+        <v>19968</v>
+      </c>
+      <c r="D26" s="30">
+        <v>2135</v>
+      </c>
+      <c r="E26" s="30">
+        <v>17833</v>
+      </c>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="5"/>
+      <c r="C30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f>CONCATENATE(B30, " &amp; ", C30, " &amp; ", D30, " &amp; ", E30, " \\ ")</f>
+        <v xml:space="preserve"> &amp; Total &amp; Wildfire Days &amp; Non-Wildfire Days \\ </v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="8">
         <v>277</v>
       </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="H9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D31" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f>CONCATENATE(B31, " &amp; ", C31, " &amp; ", D31, " &amp; ", E31, " \\ ")</f>
+        <v xml:space="preserve">Number of Days &amp; 277 &amp; 31 (16.8 - 43.2) &amp; 246 (233.8 - 260.2) \\ </v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="2" t="str">
+        <f t="shared" ref="F32:F38" si="0">CONCATENATE(B32, " &amp; ", C32, " &amp; ", D32, " &amp; ", E32, " \\ ")</f>
+        <v xml:space="preserve">Daily PM2.5 (\mu g/m^3) &amp; 5.5 (2.0 - 35.4) &amp; 26.4 (4.8 - 195.8) &amp; 5.0 (1.9 - 15.9) \\ </v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f t="shared" ref="F33:F34" si="1">CONCATENATE(B33, " &amp; ", C33, " &amp; ", D33, " &amp; ", E33, " \\ ")</f>
+        <v xml:space="preserve">Percent of Days with zero COVID19 case &amp; 26.5 (13.5 - 45.1) &amp; 23.6 (4.8 - 36.7) &amp; 27.1 (13.7 - 46.6) \\ </v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Percent of Days with zero COVID19 death &amp; 87.7(63.6 - 95.1) &amp; 84.6 (56.2 - 98.8) &amp; 88.7 (65.3 - 95.7) \\ </v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Percent of Days with zero COVID19 case &amp; 26.5% (13.5% - 45.1%) &amp; 23.6% (4.8% - 36.7%) &amp; 27.1% (13.7% - 46.6%) \\ </v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Percent of Days with zero COVID19 death &amp; 87.7%(63.6% - 95.1%) &amp; 84.6% (56.2% - 98.8%) &amp; 88.7% (65.3% - 95.7%) \\ </v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Daily Cases Rate (per 100,000) &amp; 9.8 (7.3 - 15.9) &amp; 7.9 (3.9 - 13.7) &amp; 10.0 (7.3 - 16.0) \\ </v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Daily Deaths Rate (per 1,000,000) &amp; 1.23 (0.42 - 3.05) &amp; 1.25 (0.00 - 5.91) &amp; 1.13 (0.44 - 2.96) \\ </v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="36"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="2:6" s="23" customFormat="1">
+      <c r="B40" s="28"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="2:6" s="23" customFormat="1">
+      <c r="B41" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" s="23" customFormat="1">
+      <c r="B42" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" s="23" customFormat="1">
+      <c r="B43" s="28"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+    </row>
+    <row r="44" spans="2:6" s="23" customFormat="1">
+      <c r="B44" s="28"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+    </row>
+    <row r="45" spans="2:6" s="23" customFormat="1">
+      <c r="B45" s="28"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+    </row>
+    <row r="46" spans="2:6" s="23" customFormat="1">
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+    </row>
+    <row r="47" spans="2:6" s="23" customFormat="1">
+      <c r="B47" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" s="23" customFormat="1">
+      <c r="B48" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" s="23" customFormat="1">
+      <c r="B49" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" s="23" customFormat="1">
+      <c r="B50" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="21"/>
+      <c r="F52" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>